<commit_message>
added entry for matrix stm file
</commit_message>
<xml_diff>
--- a/test/lab_journal.xlsx
+++ b/test/lab_journal.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="43">
   <si>
     <t xml:space="preserve">day</t>
   </si>
@@ -137,6 +137,18 @@
   </si>
   <si>
     <t xml:space="preserve">XPS omicron EIS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24.07.2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20201111--4_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Au(111)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Omicron Matrix File</t>
   </si>
 </sst>
 </file>
@@ -287,10 +299,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
+      <selection pane="bottomLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20"/>
@@ -589,8 +601,22 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="2"/>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="2"/>
@@ -756,18 +782,18 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="false" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="B2" type="none">
+    <dataValidation allowBlank="false" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="B2" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B1" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B1" type="whole">
       <formula1>0</formula1>
       <formula2>999</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
implementation of flm file format and automatic conversion to mp4
</commit_message>
<xml_diff>
--- a/test/lab_journal.xlsx
+++ b/test/lab_journal.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="47">
   <si>
     <t xml:space="preserve">day</t>
   </si>
@@ -149,6 +149,18 @@
   </si>
   <si>
     <t xml:space="preserve">Omicron Matrix File</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12.08.2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06a_16m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">flm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aarhus flm file</t>
   </si>
 </sst>
 </file>
@@ -299,10 +311,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
+      <selection pane="bottomLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.12890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20"/>
@@ -619,7 +631,18 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="2"/>
+      <c r="A16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="2"/>

</xml_diff>

<commit_message>
implemented Quarty Microbalance log-files
</commit_message>
<xml_diff>
--- a/test/lab_journal.xlsx
+++ b/test/lab_journal.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="51">
   <si>
     <t xml:space="preserve">day</t>
   </si>
@@ -161,6 +161,18 @@
   </si>
   <si>
     <t xml:space="preserve">Aarhus flm file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26.08.2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qcmb_test.log</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qcmb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STM2 QCMB Controller log-file</t>
   </si>
 </sst>
 </file>
@@ -311,7 +323,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+      <selection pane="bottomLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.12890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -645,7 +657,18 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="2"/>
+      <c r="A17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="2"/>

</xml_diff>